<commit_message>
Paginate the student marks records
</commit_message>
<xml_diff>
--- a/backend/InstaLearn/src/main/resources/upload/Book3.xlsx
+++ b/backend/InstaLearn/src/main/resources/upload/Book3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GroupProject\InstaLearn\backend\InstaLearn\src\main\resources\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33E5706A-4BD5-41F5-980E-BBD45A17A81F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0483651-AF03-483C-A9F6-AFEA6A06177D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{310B7804-88B9-452F-8D25-EF3CD8B69033}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>marks</t>
   </si>
@@ -47,16 +47,19 @@
     <t>studentId</t>
   </si>
   <si>
-    <t>January</t>
-  </si>
-  <si>
     <t>st45</t>
   </si>
   <si>
-    <t>February</t>
-  </si>
-  <si>
     <t>st55</t>
+  </si>
+  <si>
+    <t>st65</t>
+  </si>
+  <si>
+    <t>st75</t>
+  </si>
+  <si>
+    <t>st85</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36EF21CC-72DE-4797-80D2-3D297D8D8D7F}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,22 +454,55 @@
       <c r="A2">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>55</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>45</v>
+      </c>
+      <c r="B4">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>69</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>56</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>